<commit_message>
Updating README to reference https://github.com/luckylinux/solar-charger-emerson for updated Rootless CANbus use.
</commit_message>
<xml_diff>
--- a/strategy/2024-04-01.xlsx
+++ b/strategy/2024-04-01.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -873,7 +873,7 @@
         <v>45383.7083217593</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>54.2</v>
+        <v>55.2</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1012,7 +1012,7 @@
         <v>45383.9166550926</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>54.2</v>
+        <v>57</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1039,11 +1039,10 @@
         <v>45383.9583217593</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>54.2</v>
+        <v>54.4</v>
       </c>
       <c r="H25" s="1" t="n">
-        <f aca="false">$H$3</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,11 +1065,10 @@
         <v>45383.9999884259</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>54.2</v>
+        <v>54.4</v>
       </c>
       <c r="H26" s="1" t="n">
-        <f aca="false">$H$3</f>
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>